<commit_message>
alu address calculation synchronized with the clock.
still need to work...
</commit_message>
<xml_diff>
--- a/doc/mos6502-bus.xlsx
+++ b/doc/mos6502-bus.xlsx
@@ -1512,80 +1512,80 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>142873</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>35717</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="左右矢印 34"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10620373" y="4810125"/>
+          <a:ext cx="416719" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftRightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>130968</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>35718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="右矢印 34"/>
+      <xdr:colOff>83342</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>59531</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="左右矢印 35"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8486775" y="1714500"/>
-          <a:ext cx="257175" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="右矢印 35"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="10739438" y="7810500"/>
-          <a:ext cx="261937" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
+          <a:off x="10608468" y="7846218"/>
+          <a:ext cx="476249" cy="214313"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -4434,7 +4434,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="AH50" sqref="AH50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.375" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
reset recovery bug fix. still more refactoring needed....
</commit_message>
<xml_diff>
--- a/doc/mos6502-bus.xlsx
+++ b/doc/mos6502-bus.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\999.my-proj\001.nes-fpga\repo\motonesfpga\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="22635" windowHeight="11655"/>
   </bookViews>
@@ -16,19 +21,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -62,10 +67,18 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -73,15 +86,67 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>123392</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="右矢印 73"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2714625" y="6858000"/>
+          <a:ext cx="1028267" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -145,13 +210,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -215,13 +280,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -285,13 +350,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -337,13 +402,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -407,13 +472,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -477,13 +542,13 @@
     <xdr:from>
       <xdr:col>43</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -547,13 +612,13 @@
     <xdr:from>
       <xdr:col>32</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -617,13 +682,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -687,13 +752,13 @@
     <xdr:from>
       <xdr:col>32</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -757,13 +822,13 @@
     <xdr:from>
       <xdr:col>48</xdr:col>
       <xdr:colOff>157162</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>62</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -813,13 +878,13 @@
     <xdr:from>
       <xdr:col>43</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>119066</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -865,13 +930,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -922,13 +987,13 @@
     <xdr:from>
       <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -974,13 +1039,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1026,13 +1091,13 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1078,13 +1143,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>85724</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1130,13 +1195,13 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1182,13 +1247,13 @@
     <xdr:from>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1239,13 +1304,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>261936</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>-1</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1296,13 +1361,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1353,13 +1418,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1410,13 +1475,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1462,13 +1527,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1514,13 +1579,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>142873</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>35717</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1566,13 +1631,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>130968</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>35718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>83342</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>59531</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1618,13 +1683,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1670,13 +1735,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1722,13 +1787,13 @@
     <xdr:from>
       <xdr:col>49</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>53</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1779,13 +1844,13 @@
     <xdr:from>
       <xdr:col>50</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>50</xdr:col>
       <xdr:colOff>261936</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1831,13 +1896,13 @@
     <xdr:from>
       <xdr:col>44</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1883,13 +1948,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1940,13 +2005,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1992,13 +2057,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2044,13 +2109,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2096,13 +2161,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2153,13 +2218,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2205,13 +2270,13 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2257,13 +2322,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2314,13 +2379,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2366,13 +2431,13 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2418,13 +2483,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>190498</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2475,13 +2540,13 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2527,13 +2592,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2579,13 +2644,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2636,13 +2701,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2688,13 +2753,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>119065</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>119065</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2743,15 +2808,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>74604</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2761,8 +2826,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2357438" y="7429500"/>
-          <a:ext cx="785812" cy="2476500"/>
+          <a:off x="1131094" y="6170604"/>
+          <a:ext cx="1357313" cy="3163896"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2813,119 +2878,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="63" name="右矢印 62"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3405188" y="7620000"/>
-          <a:ext cx="785812" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="64" name="右矢印 63"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3405188" y="9525000"/>
-          <a:ext cx="785812" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2989,13 +2950,13 @@
     <xdr:from>
       <xdr:col>32</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3045,13 +3006,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3102,13 +3063,13 @@
     <xdr:from>
       <xdr:col>56</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>60</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3159,13 +3120,13 @@
     <xdr:from>
       <xdr:col>54</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>55</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3211,13 +3172,13 @@
     <xdr:from>
       <xdr:col>54</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>55</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3263,13 +3224,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3315,13 +3276,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3367,13 +3328,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3419,13 +3380,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3475,13 +3436,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3527,13 +3488,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3579,13 +3540,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3631,13 +3592,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3683,13 +3644,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3735,13 +3696,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3787,13 +3748,13 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3844,13 +3805,13 @@
     <xdr:from>
       <xdr:col>24</xdr:col>
       <xdr:colOff>257169</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>50</xdr:col>
       <xdr:colOff>258531</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3905,13 +3866,13 @@
     <xdr:from>
       <xdr:col>49</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>53</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3962,13 +3923,13 @@
     <xdr:from>
       <xdr:col>46</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
       <xdr:colOff>119059</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>71436</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4014,13 +3975,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4071,13 +4032,13 @@
     <xdr:from>
       <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4089,6 +4050,58 @@
         <a:xfrm flipH="1">
           <a:off x="10739438" y="5631658"/>
           <a:ext cx="261937" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>123392</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="右矢印 73"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2714625" y="8953500"/>
+          <a:ext cx="1028267" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -4430,16 +4443,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AH50" sqref="AH50"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.375" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="8" max="8" width="3.375" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1"/>
@@ -4449,12 +4462,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4462,12 +4475,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bus pin restored... lol!
</commit_message>
<xml_diff>
--- a/doc/mos6502-bus.xlsx
+++ b/doc/mos6502-bus.xlsx
@@ -2128,7 +2128,7 @@
           <a:off x="6810375" y="7810500"/>
           <a:ext cx="4191000" cy="190500"/>
         </a:xfrm>
-        <a:prstGeom prst="rightArrow">
+        <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -2237,7 +2237,7 @@
           <a:off x="9315451" y="1524000"/>
           <a:ext cx="714374" cy="190500"/>
         </a:xfrm>
-        <a:prstGeom prst="rightArrow">
+        <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -2398,7 +2398,7 @@
           <a:off x="9315451" y="571500"/>
           <a:ext cx="714374" cy="190500"/>
         </a:xfrm>
-        <a:prstGeom prst="rightArrow">
+        <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -2611,7 +2611,7 @@
           <a:off x="10272714" y="2476500"/>
           <a:ext cx="728661" cy="190500"/>
         </a:xfrm>
-        <a:prstGeom prst="rightArrow">
+        <a:prstGeom prst="leftRightArrow">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
@@ -4446,8 +4446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BI33" sqref="BI33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
fucking big survery still under working...
</commit_message>
<xml_diff>
--- a/doc/mos6502-bus.xlsx
+++ b/doc/mos6502-bus.xlsx
@@ -4596,14 +4596,14 @@
     <xdr:from>
       <xdr:col>32</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4612,8 +4612,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7239000" y="3048001"/>
-          <a:ext cx="226219" cy="1333500"/>
+          <a:off x="7450667" y="762001"/>
+          <a:ext cx="232833" cy="2476500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6528,14 +6528,14 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>2379</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>226217</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6544,8 +6544,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5657848" y="2095501"/>
-          <a:ext cx="2259807" cy="190500"/>
+          <a:off x="5823212" y="571500"/>
+          <a:ext cx="2319338" cy="190500"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -7540,7 +7540,7 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -7556,8 +7556,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6334125" y="5334000"/>
-          <a:ext cx="226219" cy="3429000"/>
+          <a:off x="6519333" y="2667000"/>
+          <a:ext cx="232834" cy="2476500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7853,6 +7853,58 @@
               <a:schemeClr val="tx1"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="右矢印 70"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5820833" y="952500"/>
+          <a:ext cx="1397000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -8192,7 +8244,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="AE16" sqref="AE16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
test and doc update
</commit_message>
<xml_diff>
--- a/doc/mos6502-bus.xlsx
+++ b/doc/mos6502-bus.xlsx
@@ -4142,13 +4142,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>123392</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4194,13 +4194,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4264,13 +4264,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4334,13 +4334,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4404,13 +4404,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2381</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4456,13 +4456,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>3</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>35718</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4526,13 +4526,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>2</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4596,13 +4596,13 @@
     <xdr:from>
       <xdr:col>32</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4666,13 +4666,13 @@
     <xdr:from>
       <xdr:col>27</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>53</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4721,13 +4721,13 @@
     <xdr:from>
       <xdr:col>43</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>119066</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4773,13 +4773,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4830,13 +4830,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>107158</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4882,13 +4882,13 @@
     <xdr:from>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4939,13 +4939,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4996,13 +4996,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5053,13 +5053,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>2380</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>2381</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5105,13 +5105,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5157,13 +5157,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>142873</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>119063</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>35717</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>119063</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5209,13 +5209,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>130968</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>35718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>83342</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>59531</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5261,13 +5261,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5313,13 +5313,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5365,13 +5365,13 @@
     <xdr:from>
       <xdr:col>48</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5422,13 +5422,13 @@
     <xdr:from>
       <xdr:col>49</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>50</xdr:col>
       <xdr:colOff>3740</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5474,13 +5474,13 @@
     <xdr:from>
       <xdr:col>44</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
       <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5526,13 +5526,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>16920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>173581</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5583,13 +5583,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5640,13 +5640,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5692,13 +5692,13 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5744,13 +5744,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5801,13 +5801,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5853,13 +5853,13 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5905,13 +5905,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>190498</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -5962,13 +5962,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>57151</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6014,13 +6014,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>107159</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6071,13 +6071,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6123,13 +6123,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>119065</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6180,13 +6180,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>16180</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>174321</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6257,13 +6257,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>2380</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>2380</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6302,7 +6302,15 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
-            <a:t>addr calc</a:t>
+            <a:t>Address</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2000"/>
+            <a:t>Calcurator</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2000"/>
         </a:p>
@@ -6314,13 +6322,13 @@
     <xdr:from>
       <xdr:col>55</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>59</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6371,13 +6379,13 @@
     <xdr:from>
       <xdr:col>53</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>54</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6423,13 +6431,13 @@
     <xdr:from>
       <xdr:col>53</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>54</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6475,13 +6483,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6527,13 +6535,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>2379</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
       <xdr:colOff>226217</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6579,13 +6587,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6631,13 +6639,13 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>2</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>3</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6683,13 +6691,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6735,13 +6743,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>2379</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>2381</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6787,13 +6795,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6839,13 +6847,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6891,13 +6899,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>2375</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>50</xdr:col>
       <xdr:colOff>3738</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -6952,13 +6960,13 @@
     <xdr:from>
       <xdr:col>48</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7009,13 +7017,13 @@
     <xdr:from>
       <xdr:col>43</xdr:col>
       <xdr:colOff>31882</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>96388</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>84665</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7061,13 +7069,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7118,13 +7126,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>123392</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7171,13 +7179,13 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7186,8 +7194,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2940844" y="1523999"/>
-          <a:ext cx="2488406" cy="952501"/>
+          <a:off x="3026833" y="381000"/>
+          <a:ext cx="2561167" cy="1524001"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7227,13 +7235,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>142873</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>95248</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>35717</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>95248</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7279,13 +7287,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>154782</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>83342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>47626</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>83342</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7331,13 +7339,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>83342</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>83342</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7383,13 +7391,13 @@
     <xdr:from>
       <xdr:col>40</xdr:col>
       <xdr:colOff>154782</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
       <xdr:colOff>47626</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7435,13 +7443,13 @@
     <xdr:from>
       <xdr:col>30</xdr:col>
       <xdr:colOff>2380</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>35718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>2381</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>35718</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7487,13 +7495,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7539,13 +7547,13 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7609,13 +7617,13 @@
     <xdr:from>
       <xdr:col>26</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>59531</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7679,13 +7687,13 @@
     <xdr:from>
       <xdr:col>21</xdr:col>
       <xdr:colOff>91675</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>190498</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>2379</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7741,7 +7749,7 @@
     <xdr:to>
       <xdr:col>44</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7751,8 +7759,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9727406" y="1524001"/>
-          <a:ext cx="226219" cy="9143999"/>
+          <a:off x="10011833" y="571501"/>
+          <a:ext cx="232834" cy="6286499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7805,13 +7813,13 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>35718</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7861,13 +7869,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>31</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7914,13 +7922,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>62</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7929,8 +7937,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="931333" y="190500"/>
-          <a:ext cx="13737167" cy="8001000"/>
+          <a:off x="931333" y="190501"/>
+          <a:ext cx="13504334" cy="8382000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -7965,6 +7973,58 @@
             <a:rPr kumimoji="1" lang="en-US" sz="1800"/>
             <a:t>MOS 6502 CPU</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>232832</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>232832</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="右矢印 56"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5820832" y="730250"/>
+          <a:ext cx="3958167" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftRightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -8303,8 +8363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W48" sqref="W48"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
alu clean up, clock synchronized.
</commit_message>
<xml_diff>
--- a/doc/mos6502-bus.xlsx
+++ b/doc/mos6502-bus.xlsx
@@ -5905,14 +5905,14 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>190498</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5921,8 +5921,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8143875" y="1523999"/>
-          <a:ext cx="452438" cy="952499"/>
+          <a:off x="8382000" y="1143001"/>
+          <a:ext cx="465667" cy="571499"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7178,7 +7178,7 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -7194,8 +7194,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3026833" y="381000"/>
-          <a:ext cx="2561167" cy="1524001"/>
+          <a:off x="3026833" y="571500"/>
+          <a:ext cx="2561167" cy="1333501"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8364,7 +8364,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="BO25" sqref="BO25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
reset vector position change
</commit_message>
<xml_diff>
--- a/doc/mos6502-bus.xlsx
+++ b/doc/mos6502-bus.xlsx
@@ -4140,58 +4140,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>123392</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="右矢印 73"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2714625" y="4762500"/>
-          <a:ext cx="1028267" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
@@ -6178,83 +6126,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>228599</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>16180</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>174321</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="正方形/長方形 60"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1625599" y="4588180"/>
-          <a:ext cx="935569" cy="1301141"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent4"/>
-        </a:fillRef>
-        <a:effectRef idx="3">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400"/>
-            <a:t>Reset</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400"/>
-            <a:t>NMI</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400"/>
-            <a:t>IRQ</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400"/>
-            <a:t>Vector</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>2380</xdr:colOff>
       <xdr:row>11</xdr:row>
@@ -7116,58 +6987,6 @@
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
             <a:t>IDL_L</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>123392</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="73" name="右矢印 73"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2714625" y="5524500"/>
-          <a:ext cx="1028267" cy="190500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -8024,6 +7843,69 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>34130</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>21165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38363</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>21165</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="正方形/長方形 60"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3060963" y="2116665"/>
+          <a:ext cx="702733" cy="571500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" vert="horz" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Reset</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>Vector</a:t>
+          </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -8363,8 +8245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="BO25" sqref="BO25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>